<commit_message>
Update scatter and clustering plot
</commit_message>
<xml_diff>
--- a/artifacts/python-scripts/distance/distances.xlsx
+++ b/artifacts/python-scripts/distance/distances.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,35 +481,40 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>CoSim20</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>UMoC++</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>LinguaFranca</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Reo</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Linda</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>BIP</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Manifold</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>ForSyDe</t>
         </is>
@@ -538,30 +543,33 @@
         <v>0.5882352941176471</v>
       </c>
       <c r="H2" t="n">
-        <v>0.7894736842105263</v>
+        <v>0.8</v>
       </c>
       <c r="I2" t="n">
         <v>0.85</v>
       </c>
       <c r="J2" t="n">
+        <v>0.736842105263158</v>
+      </c>
+      <c r="K2" t="n">
         <v>0.6470588235294117</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>0.7619047619047619</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>0.6111111111111112</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>0.85</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>0.5</v>
       </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
         <v>0.7222222222222222</v>
       </c>
-      <c r="P2" t="n">
+      <c r="Q2" t="n">
         <v>0.7</v>
       </c>
     </row>
@@ -588,30 +596,33 @@
         <v>0.6666666666666667</v>
       </c>
       <c r="H3" t="n">
-        <v>0.7894736842105263</v>
+        <v>0.8</v>
       </c>
       <c r="I3" t="n">
         <v>0.85</v>
       </c>
       <c r="J3" t="n">
+        <v>0.736842105263158</v>
+      </c>
+      <c r="K3" t="n">
         <v>0.6470588235294117</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>0.7619047619047619</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>0.5294117647058824</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>0.85</v>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>0.5</v>
       </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
         <v>0.7222222222222222</v>
       </c>
-      <c r="P3" t="n">
+      <c r="Q3" t="n">
         <v>0.7</v>
       </c>
     </row>
@@ -638,30 +649,33 @@
         <v>0.4705882352941176</v>
       </c>
       <c r="H4" t="n">
-        <v>0.4375</v>
+        <v>0.4705882352941176</v>
       </c>
       <c r="I4" t="n">
         <v>0.5294117647058824</v>
       </c>
       <c r="J4" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="K4" t="n">
         <v>0.4375</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>0.5263157894736843</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>0.4117647058823529</v>
       </c>
-      <c r="M4" t="n">
+      <c r="N4" t="n">
         <v>0.75</v>
       </c>
-      <c r="N4" t="n">
+      <c r="O4" t="n">
         <v>0.4736842105263158</v>
       </c>
-      <c r="O4" t="n">
+      <c r="P4" t="n">
         <v>0.5294117647058824</v>
       </c>
-      <c r="P4" t="n">
+      <c r="Q4" t="n">
         <v>0.4444444444444444</v>
       </c>
     </row>
@@ -688,30 +702,33 @@
         <v>0.5294117647058824</v>
       </c>
       <c r="H5" t="n">
-        <v>0.8</v>
+        <v>0.8095238095238095</v>
       </c>
       <c r="I5" t="n">
         <v>0.736842105263158</v>
       </c>
       <c r="J5" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="K5" t="n">
         <v>0.5</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>0.65</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
         <v>0.2666666666666667</v>
       </c>
-      <c r="M5" t="n">
+      <c r="N5" t="n">
         <v>0.8</v>
       </c>
-      <c r="N5" t="n">
+      <c r="O5" t="n">
         <v>0.25</v>
       </c>
-      <c r="O5" t="n">
+      <c r="P5" t="n">
         <v>0.5882352941176471</v>
       </c>
-      <c r="P5" t="n">
+      <c r="Q5" t="n">
         <v>0.5789473684210527</v>
       </c>
     </row>
@@ -738,30 +755,33 @@
         <v>0.2857142857142857</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6470588235294117</v>
+        <v>0.6666666666666667</v>
       </c>
       <c r="I6" t="n">
         <v>0.5625</v>
       </c>
       <c r="J6" t="n">
+        <v>0.5882352941176471</v>
+      </c>
+      <c r="K6" t="n">
         <v>0.2307692307692307</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>0.2666666666666667</v>
       </c>
-      <c r="L6" t="n">
+      <c r="M6" t="n">
         <v>0.3333333333333334</v>
       </c>
-      <c r="M6" t="n">
+      <c r="N6" t="n">
         <v>0.4666666666666667</v>
       </c>
-      <c r="N6" t="n">
+      <c r="O6" t="n">
         <v>0.4117647058823529</v>
       </c>
-      <c r="O6" t="n">
+      <c r="P6" t="n">
         <v>0.3571428571428571</v>
       </c>
-      <c r="P6" t="n">
+      <c r="Q6" t="n">
         <v>0.2666666666666667</v>
       </c>
     </row>
@@ -788,30 +808,33 @@
         <v>0.2857142857142857</v>
       </c>
       <c r="H7" t="n">
-        <v>0.6470588235294117</v>
+        <v>0.6666666666666667</v>
       </c>
       <c r="I7" t="n">
         <v>0.5625</v>
       </c>
       <c r="J7" t="n">
+        <v>0.5882352941176471</v>
+      </c>
+      <c r="K7" t="n">
         <v>0.2307692307692307</v>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>0.4705882352941176</v>
       </c>
-      <c r="L7" t="n">
+      <c r="M7" t="n">
         <v>0.2142857142857143</v>
       </c>
-      <c r="M7" t="n">
+      <c r="N7" t="n">
         <v>0.6470588235294117</v>
       </c>
-      <c r="N7" t="n">
+      <c r="O7" t="n">
         <v>0.3125</v>
       </c>
-      <c r="O7" t="n">
+      <c r="P7" t="n">
         <v>0.3571428571428571</v>
       </c>
-      <c r="P7" t="n">
+      <c r="Q7" t="n">
         <v>0.375</v>
       </c>
     </row>
@@ -838,81 +861,87 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>0.5625</v>
+        <v>0.5882352941176471</v>
       </c>
       <c r="I8" t="n">
         <v>0.4666666666666667</v>
       </c>
       <c r="J8" t="n">
+        <v>0.5882352941176471</v>
+      </c>
+      <c r="K8" t="n">
         <v>0.08333333333333337</v>
       </c>
-      <c r="K8" t="n">
+      <c r="L8" t="n">
         <v>0.4705882352941176</v>
       </c>
-      <c r="L8" t="n">
+      <c r="M8" t="n">
         <v>0.3333333333333334</v>
       </c>
-      <c r="M8" t="n">
+      <c r="N8" t="n">
         <v>0.5625</v>
       </c>
-      <c r="N8" t="n">
+      <c r="O8" t="n">
         <v>0.4117647058823529</v>
       </c>
-      <c r="O8" t="n">
+      <c r="P8" t="n">
         <v>0.2307692307692307</v>
       </c>
-      <c r="P8" t="n">
+      <c r="Q8" t="n">
         <v>0.4705882352941176</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.7894736842105263</v>
+        <v>0.8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.7894736842105263</v>
+        <v>0.8</v>
       </c>
       <c r="C9" t="n">
-        <v>0.4375</v>
+        <v>0.4705882352941176</v>
       </c>
       <c r="D9" t="n">
-        <v>0.8</v>
+        <v>0.8095238095238095</v>
       </c>
       <c r="E9" t="n">
+        <v>0.6666666666666667</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.6666666666666667</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.5882352941176471</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.2307692307692307</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.1538461538461539</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.5625</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.631578947368421</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.6842105263157895</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.7222222222222222</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="P9" t="n">
         <v>0.6470588235294117</v>
       </c>
-      <c r="F9" t="n">
-        <v>0.6470588235294117</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.5625</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.1666666666666666</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.5333333333333333</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.6111111111111112</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0.6666666666666667</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0.7058823529411764</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="O9" t="n">
-        <v>0.625</v>
-      </c>
-      <c r="P9" t="n">
-        <v>0.75</v>
+      <c r="Q9" t="n">
+        <v>0.7619047619047619</v>
       </c>
     </row>
     <row r="10">
@@ -938,380 +967,457 @@
         <v>0.4666666666666667</v>
       </c>
       <c r="H10" t="n">
-        <v>0.1666666666666666</v>
+        <v>0.2307692307692307</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
       </c>
       <c r="J10" t="n">
+        <v>0.2307692307692307</v>
+      </c>
+      <c r="K10" t="n">
         <v>0.4285714285714286</v>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>0.5294117647058824</v>
       </c>
-      <c r="L10" t="n">
+      <c r="M10" t="n">
         <v>0.5882352941176471</v>
       </c>
-      <c r="M10" t="n">
+      <c r="N10" t="n">
         <v>0.625</v>
       </c>
-      <c r="N10" t="n">
+      <c r="O10" t="n">
         <v>0.631578947368421</v>
       </c>
-      <c r="O10" t="n">
+      <c r="P10" t="n">
         <v>0.5333333333333333</v>
       </c>
-      <c r="P10" t="n">
+      <c r="Q10" t="n">
         <v>0.6842105263157895</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
+        <v>0.736842105263158</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.736842105263158</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.5882352941176471</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.5882352941176471</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.5882352941176471</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.1538461538461539</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.2307692307692307</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.5625</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.6111111111111112</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.7222222222222222</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="P11" t="n">
         <v>0.6470588235294117</v>
       </c>
-      <c r="B11" t="n">
-        <v>0.6470588235294117</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.4375</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.2307692307692307</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.2307692307692307</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.08333333333333337</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.5333333333333333</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.4285714285714286</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0.4375</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0.5333333333333333</v>
-      </c>
-      <c r="N11" t="n">
-        <v>0.375</v>
-      </c>
-      <c r="O11" t="n">
-        <v>0.1666666666666666</v>
-      </c>
-      <c r="P11" t="n">
-        <v>0.4375</v>
+      <c r="Q11" t="n">
+        <v>0.7</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.7619047619047619</v>
+        <v>0.6470588235294117</v>
       </c>
       <c r="B12" t="n">
-        <v>0.7619047619047619</v>
+        <v>0.6470588235294117</v>
       </c>
       <c r="C12" t="n">
-        <v>0.5263157894736843</v>
+        <v>0.4375</v>
       </c>
       <c r="D12" t="n">
-        <v>0.65</v>
+        <v>0.5</v>
       </c>
       <c r="E12" t="n">
-        <v>0.2666666666666667</v>
+        <v>0.2307692307692307</v>
       </c>
       <c r="F12" t="n">
-        <v>0.4705882352941176</v>
+        <v>0.2307692307692307</v>
       </c>
       <c r="G12" t="n">
-        <v>0.4705882352941176</v>
+        <v>0.08333333333333337</v>
       </c>
       <c r="H12" t="n">
-        <v>0.6111111111111112</v>
+        <v>0.5625</v>
       </c>
       <c r="I12" t="n">
-        <v>0.5294117647058824</v>
+        <v>0.4285714285714286</v>
       </c>
       <c r="J12" t="n">
+        <v>0.5625</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
         <v>0.4375</v>
       </c>
-      <c r="K12" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0.5</v>
-      </c>
       <c r="M12" t="n">
-        <v>0.3333333333333334</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="N12" t="n">
-        <v>0.4736842105263158</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="O12" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.1666666666666666</v>
+      </c>
+      <c r="Q12" t="n">
         <v>0.4375</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0.25</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.6111111111111112</v>
+        <v>0.7619047619047619</v>
       </c>
       <c r="B13" t="n">
+        <v>0.7619047619047619</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.5263157894736843</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.2666666666666667</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.4705882352941176</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.4705882352941176</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.631578947368421</v>
+      </c>
+      <c r="I13" t="n">
         <v>0.5294117647058824</v>
       </c>
-      <c r="C13" t="n">
-        <v>0.4117647058823529</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.2666666666666667</v>
-      </c>
-      <c r="E13" t="n">
+      <c r="J13" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.4375</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N13" t="n">
         <v>0.3333333333333334</v>
       </c>
-      <c r="F13" t="n">
-        <v>0.2142857142857143</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.3333333333333334</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.6666666666666667</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0.5882352941176471</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0.6666666666666667</v>
-      </c>
-      <c r="N13" t="n">
-        <v>0.3529411764705882</v>
-      </c>
       <c r="O13" t="n">
-        <v>0.4</v>
+        <v>0.4736842105263158</v>
       </c>
       <c r="P13" t="n">
-        <v>0.4117647058823529</v>
+        <v>0.4375</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.25</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.85</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="B14" t="n">
-        <v>0.85</v>
+        <v>0.5294117647058824</v>
       </c>
       <c r="C14" t="n">
-        <v>0.75</v>
+        <v>0.4117647058823529</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8</v>
+        <v>0.2666666666666667</v>
       </c>
       <c r="E14" t="n">
-        <v>0.4666666666666667</v>
+        <v>0.3333333333333334</v>
       </c>
       <c r="F14" t="n">
-        <v>0.6470588235294117</v>
+        <v>0.2142857142857143</v>
       </c>
       <c r="G14" t="n">
-        <v>0.5625</v>
+        <v>0.3333333333333334</v>
       </c>
       <c r="H14" t="n">
-        <v>0.7058823529411764</v>
+        <v>0.6842105263157895</v>
       </c>
       <c r="I14" t="n">
-        <v>0.625</v>
+        <v>0.5882352941176471</v>
       </c>
       <c r="J14" t="n">
-        <v>0.5333333333333333</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="K14" t="n">
-        <v>0.3333333333333334</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="L14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
         <v>0.6666666666666667</v>
       </c>
-      <c r="M14" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" t="n">
-        <v>0.631578947368421</v>
-      </c>
       <c r="O14" t="n">
-        <v>0.4285714285714286</v>
+        <v>0.3529411764705882</v>
       </c>
       <c r="P14" t="n">
-        <v>0.4375</v>
+        <v>0.4</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.4117647058823529</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.5</v>
+        <v>0.85</v>
       </c>
       <c r="B15" t="n">
-        <v>0.5</v>
+        <v>0.85</v>
       </c>
       <c r="C15" t="n">
-        <v>0.4736842105263158</v>
+        <v>0.75</v>
       </c>
       <c r="D15" t="n">
-        <v>0.25</v>
+        <v>0.8</v>
       </c>
       <c r="E15" t="n">
-        <v>0.4117647058823529</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="F15" t="n">
-        <v>0.3125</v>
+        <v>0.6470588235294117</v>
       </c>
       <c r="G15" t="n">
-        <v>0.4117647058823529</v>
+        <v>0.5625</v>
       </c>
       <c r="H15" t="n">
-        <v>0.7</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="I15" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.7222222222222222</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.5333333333333333</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.3333333333333334</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.6666666666666667</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
         <v>0.631578947368421</v>
       </c>
-      <c r="J15" t="n">
-        <v>0.375</v>
-      </c>
-      <c r="K15" t="n">
-        <v>0.4736842105263158</v>
-      </c>
-      <c r="L15" t="n">
-        <v>0.3529411764705882</v>
-      </c>
-      <c r="M15" t="n">
-        <v>0.631578947368421</v>
-      </c>
-      <c r="N15" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" t="n">
-        <v>0.375</v>
-      </c>
       <c r="P15" t="n">
-        <v>0.3888888888888888</v>
+        <v>0.4285714285714286</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.4375</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.5</v>
       </c>
       <c r="B16" t="n">
-        <v>0.7222222222222222</v>
+        <v>0.5</v>
       </c>
       <c r="C16" t="n">
-        <v>0.5294117647058824</v>
+        <v>0.4736842105263158</v>
       </c>
       <c r="D16" t="n">
-        <v>0.5882352941176471</v>
+        <v>0.25</v>
       </c>
       <c r="E16" t="n">
-        <v>0.3571428571428571</v>
+        <v>0.4117647058823529</v>
       </c>
       <c r="F16" t="n">
-        <v>0.3571428571428571</v>
+        <v>0.3125</v>
       </c>
       <c r="G16" t="n">
-        <v>0.2307692307692307</v>
+        <v>0.4117647058823529</v>
       </c>
       <c r="H16" t="n">
-        <v>0.625</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="I16" t="n">
-        <v>0.5333333333333333</v>
+        <v>0.631578947368421</v>
       </c>
       <c r="J16" t="n">
-        <v>0.1666666666666666</v>
+        <v>0.65</v>
       </c>
       <c r="K16" t="n">
-        <v>0.4375</v>
+        <v>0.375</v>
       </c>
       <c r="L16" t="n">
-        <v>0.4</v>
+        <v>0.4736842105263158</v>
       </c>
       <c r="M16" t="n">
-        <v>0.4285714285714286</v>
+        <v>0.3529411764705882</v>
       </c>
       <c r="N16" t="n">
+        <v>0.631578947368421</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" t="n">
         <v>0.375</v>
       </c>
-      <c r="O16" t="n">
-        <v>0</v>
-      </c>
-      <c r="P16" t="n">
-        <v>0.3333333333333334</v>
+      <c r="Q16" t="n">
+        <v>0.3888888888888888</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
+        <v>0.7222222222222222</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.7222222222222222</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.5294117647058824</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.5882352941176471</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.3571428571428571</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.3571428571428571</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.2307692307692307</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.6470588235294117</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.5333333333333333</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.6470588235294117</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.1666666666666666</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.4375</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.4285714285714286</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.3333333333333334</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
         <v>0.7</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B18" t="n">
         <v>0.7</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C18" t="n">
         <v>0.4444444444444444</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D18" t="n">
         <v>0.5789473684210527</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E18" t="n">
         <v>0.2666666666666667</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F18" t="n">
         <v>0.375</v>
       </c>
-      <c r="G17" t="n">
+      <c r="G18" t="n">
         <v>0.4705882352941176</v>
       </c>
-      <c r="H17" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="I17" t="n">
+      <c r="H18" t="n">
+        <v>0.7619047619047619</v>
+      </c>
+      <c r="I18" t="n">
         <v>0.6842105263157895</v>
       </c>
-      <c r="J17" t="n">
+      <c r="J18" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="K18" t="n">
         <v>0.4375</v>
       </c>
-      <c r="K17" t="n">
+      <c r="L18" t="n">
         <v>0.25</v>
       </c>
-      <c r="L17" t="n">
+      <c r="M18" t="n">
         <v>0.4117647058823529</v>
       </c>
-      <c r="M17" t="n">
+      <c r="N18" t="n">
         <v>0.4375</v>
       </c>
-      <c r="N17" t="n">
+      <c r="O18" t="n">
         <v>0.3888888888888888</v>
       </c>
-      <c r="O17" t="n">
+      <c r="P18" t="n">
         <v>0.3333333333333334</v>
       </c>
-      <c r="P17" t="n">
+      <c r="Q18" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>